<commit_message>
Latest Update with Validation
By Kevin Biazon
</commit_message>
<xml_diff>
--- a/documentation/Test Case.xlsx
+++ b/documentation/Test Case.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4200" windowWidth="20490" windowHeight="7740"/>
+    <workbookView xWindow="0" yWindow="5400" windowWidth="20490" windowHeight="7740"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="143">
   <si>
     <t>System Name:</t>
   </si>
@@ -254,9 +254,6 @@
     <t>1. Click Add button.</t>
   </si>
   <si>
-    <t>1. Add button has disabled.</t>
-  </si>
-  <si>
     <t>TC012_SavTypeMain_Add</t>
   </si>
   <si>
@@ -267,6 +264,195 @@
   </si>
   <si>
     <t>Savings Type Name: [Any numeric data]</t>
+  </si>
+  <si>
+    <t>1. Savings Type Name textbox will show invalid icon.</t>
+  </si>
+  <si>
+    <t>2. Add button disabled.</t>
+  </si>
+  <si>
+    <t>1. Add button disabled.</t>
+  </si>
+  <si>
+    <t>TC013_SavTypeMain_Add</t>
+  </si>
+  <si>
+    <t>Verify that user can add savings type with invalid data.</t>
+  </si>
+  <si>
+    <t>1. Enter the given data.</t>
+  </si>
+  <si>
+    <t>Maintaining Balance: [Alphanumeric data]</t>
+  </si>
+  <si>
+    <t>Max. Withdrawal Amount: [Alphanumeric data]</t>
+  </si>
+  <si>
+    <t>No. of Account Holders: [Alphanumeric data]</t>
+  </si>
+  <si>
+    <t>Interest Rate: [Alphanumeric data]</t>
+  </si>
+  <si>
+    <t>1. Any given textboxes cannot input alphabetic characters except period.</t>
+  </si>
+  <si>
+    <t>TC014_SavTypeMain_Update</t>
+  </si>
+  <si>
+    <t>Verify that user can change savings type.</t>
+  </si>
+  <si>
+    <t>1. Double click to select the savings type in the datagridview.</t>
+  </si>
+  <si>
+    <t>2. Change interest percentage to fixed</t>
+  </si>
+  <si>
+    <t>3. Click Update button.</t>
+  </si>
+  <si>
+    <t>1.Dialog will appear for confirmation.</t>
+  </si>
+  <si>
+    <t>2. The updated savings type will appear in the datagridview with update data.</t>
+  </si>
+  <si>
+    <t>TC015_SavDormMain_Add</t>
+  </si>
+  <si>
+    <t>1. Select Savings Type.</t>
+  </si>
+  <si>
+    <t>3. Choose Fixed Amount and Active.</t>
+  </si>
+  <si>
+    <t>2. Input Inactive Duration and Amount Deducted</t>
+  </si>
+  <si>
+    <t>Inactive Duration: 25</t>
+  </si>
+  <si>
+    <t>Amount Deducted: 100</t>
+  </si>
+  <si>
+    <t>TC016_SavDormMain_Update</t>
+  </si>
+  <si>
+    <t>Verify that user can update dormancy of a savings type</t>
+  </si>
+  <si>
+    <t>Verify that user can add dormancy of a savings type</t>
+  </si>
+  <si>
+    <t>1. Double click the savings type that wants to be change.</t>
+  </si>
+  <si>
+    <t>2. Change the inactivity period.</t>
+  </si>
+  <si>
+    <t>Day to month</t>
+  </si>
+  <si>
+    <t>1. Dialog box will appear. Record has been added.</t>
+  </si>
+  <si>
+    <t>2. The added record will show in the datagridview.</t>
+  </si>
+  <si>
+    <t>1. Dialog box will appear. Record has been updated.</t>
+  </si>
+  <si>
+    <t>TC017_TimeDepoTermRates_Add</t>
+  </si>
+  <si>
+    <t>1. Enter valid data.</t>
+  </si>
+  <si>
+    <t>From: 1000.00</t>
+  </si>
+  <si>
+    <t>To: 4999.00</t>
+  </si>
+  <si>
+    <t>No. of Days: 60</t>
+  </si>
+  <si>
+    <t>Interest Rate: 1.25</t>
+  </si>
+  <si>
+    <t>Status: Active</t>
+  </si>
+  <si>
+    <t>TC018_TimeDepoTermRates_Update</t>
+  </si>
+  <si>
+    <t>Verify that user can update terms and rate on the time deposit.</t>
+  </si>
+  <si>
+    <t>Verify that user can add terms and rates on the time deposit.</t>
+  </si>
+  <si>
+    <t>1. Double click the terms and rates that you want to change.</t>
+  </si>
+  <si>
+    <t>2. Change Interest rate.</t>
+  </si>
+  <si>
+    <t>2. The updated terms and Rates will appear with updated data.</t>
+  </si>
+  <si>
+    <t>TC019_TimeDepoPreTerm_Add</t>
+  </si>
+  <si>
+    <t>Verify that user can add pre termination penalty on the time deposit.</t>
+  </si>
+  <si>
+    <t>TC020_MemberType_Add</t>
+  </si>
+  <si>
+    <t>Verify that user can add Member type.</t>
+  </si>
+  <si>
+    <t>1. Enter a valid member type</t>
+  </si>
+  <si>
+    <t>Member type: Another Member</t>
+  </si>
+  <si>
+    <t>Minimum Share: 100</t>
+  </si>
+  <si>
+    <t>Checked has certificate check box</t>
+  </si>
+  <si>
+    <t>select active</t>
+  </si>
+  <si>
+    <t>TC021_MemberType_Update</t>
+  </si>
+  <si>
+    <t>Verify that user can update member type</t>
+  </si>
+  <si>
+    <t>1. Double click the member type that you want to change.</t>
+  </si>
+  <si>
+    <t>2. Change Member type name.</t>
+  </si>
+  <si>
+    <t>Member type: Kiddie Member</t>
+  </si>
+  <si>
+    <t>1. Dialog box will appear. Record had successfully updated.</t>
+  </si>
+  <si>
+    <t>2. the updated record will show in the datagridview.</t>
+  </si>
+  <si>
+    <t>TC022_</t>
   </si>
 </sst>
 </file>
@@ -599,20 +785,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:I65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A65" sqref="A65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="72" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="71.140625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="49.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="56.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="43.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="90.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6.42578125" bestFit="1" customWidth="1"/>
@@ -973,32 +1159,343 @@
         <v>75</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="C33" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D33" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C33" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D33" s="2" t="s">
+      <c r="E33" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E33" s="2" t="s">
+      <c r="F33" s="2" t="s">
         <v>80</v>
-      </c>
-      <c r="F33" s="2">
-        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D34" s="2" t="s">
         <v>70</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E36" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E37" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E38" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D40" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D41" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D43" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D44" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D46" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D47" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D49" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E50" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E51" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E52" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D54" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D55" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D57" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D59" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E60" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E61" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D63" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D64" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>